<commit_message>
up to SDR-127B done
</commit_message>
<xml_diff>
--- a/0 - Ancillary files/2019 Weir Dims.xlsx
+++ b/0 - Ancillary files/2019 Weir Dims.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Projects-South\Environmental - Schaedler\5025-19-W006 CoSDWQ TO6 Low Flow Monitoring\DATA\Data Processing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex.messina\Documents\GitHub\SD_County_LowFlow\0 - Ancillary files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="May 2019" sheetId="1" r:id="rId1"/>
+    <sheet name="ESRI_MAPINFO_SHEET" sheetId="2" state="veryHidden" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'May 2019'!$A$1:$J$67</definedName>
@@ -383,6 +384,100 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>294147</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>5045</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="EsriDoNotEdit"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="6390147" cy="1650965"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="none" lIns="91440" tIns="45720" rIns="91440" bIns="45720">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="5000" b="1" i="0" cap="none" spc="0">
+              <a:ln w="18000">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="140000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:miter lim="800000"/>
+              </a:ln>
+              <a:noFill/>
+              <a:effectLst>
+                <a:outerShdw blurRad="25500" dist="23000" dir="7020000" algn="tl">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="50000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>DO NOT EDIT </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="5000" b="1" i="0" cap="none" spc="0">
+              <a:ln w="18000">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="140000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:miter lim="800000"/>
+              </a:ln>
+              <a:noFill/>
+              <a:effectLst>
+                <a:outerShdw blurRad="25500" dist="23000" dir="7020000" algn="tl">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="50000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> For Esri use only</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -651,7 +746,8 @@
   <dimension ref="A1:L67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2739,4 +2835,17 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>